<commit_message>
Minor fixes in monthly report file
</commit_message>
<xml_diff>
--- a/test_data/Miesięczny_03.2023.xlsx
+++ b/test_data/Miesięczny_03.2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dane\Python\Wlasne\Report\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FE2AE1-A9C9-46CD-840A-BFC411CD973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB41F24-649B-4859-92ED-90CAA6ACAF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32295" yWindow="2640" windowWidth="21600" windowHeight="11295" tabRatio="710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E1" sheetId="2" r:id="rId1"/>
@@ -1453,11 +1453,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1466,35 +1483,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1503,6 +1493,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="58">
@@ -1895,11 +1895,11 @@
   </sheetPr>
   <dimension ref="A1:DV45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AB21" sqref="AB21"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,10 +1920,10 @@
       <c r="C1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="122"/>
+      <c r="E1" s="111"/>
       <c r="F1" s="103" t="s">
         <v>7</v>
       </c>
@@ -1942,28 +1942,28 @@
       <c r="K1" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="126" t="s">
+      <c r="L1" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="122"/>
+      <c r="M1" s="111"/>
       <c r="N1" s="78" t="s">
         <v>5</v>
       </c>
       <c r="O1" s="57"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="120" t="s">
+      <c r="P1" s="120"/>
+      <c r="Q1" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="119" t="s">
+      <c r="R1" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="119" t="s">
+      <c r="S1" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="119" t="s">
+      <c r="T1" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="110" t="s">
+      <c r="U1" s="119" t="s">
         <v>17</v>
       </c>
       <c r="V1" s="4"/>
@@ -2018,12 +2018,12 @@
         <v>19</v>
       </c>
       <c r="O2" s="18"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
@@ -2076,12 +2076,12 @@
         <v>24</v>
       </c>
       <c r="O3" s="18"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="111"/>
-      <c r="S3" s="111"/>
-      <c r="T3" s="111"/>
-      <c r="U3" s="111"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
@@ -2100,10 +2100,10 @@
       <c r="C4" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="124"/>
+      <c r="E4" s="113"/>
       <c r="F4" s="105" t="s">
         <v>30</v>
       </c>
@@ -2122,20 +2122,20 @@
       <c r="K4" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="123" t="s">
+      <c r="L4" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="124"/>
+      <c r="M4" s="113"/>
       <c r="N4" s="79" t="s">
         <v>57</v>
       </c>
       <c r="O4" s="57"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
+      <c r="P4" s="122"/>
+      <c r="Q4" s="117"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
+      <c r="T4" s="117"/>
+      <c r="U4" s="117"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
@@ -2166,12 +2166,12 @@
         <v>55</v>
       </c>
       <c r="O5" s="87"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
+      <c r="P5" s="123"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
     </row>
     <row r="6" spans="1:28" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89">
@@ -2195,25 +2195,25 @@
       <c r="M6" s="85"/>
       <c r="N6" s="85"/>
       <c r="O6" s="86"/>
-      <c r="P6" s="117"/>
+      <c r="P6" s="124"/>
       <c r="Q6" s="30">
-        <f>SUM(B6:P6)</f>
+        <f t="shared" ref="Q6:Q36" si="0">SUM(B6:P6)</f>
         <v>311.68</v>
       </c>
       <c r="R6" s="19">
-        <f>SUMIFS(B6:P6,B$3:P$3,"WB")</f>
+        <f t="shared" ref="R6:R36" si="1">SUMIFS(B6:P6,B$3:P$3,"WB")</f>
         <v>0</v>
       </c>
       <c r="S6" s="19">
-        <f>SUMIFS(B6:P6,B$3:P$3,"AG")</f>
+        <f t="shared" ref="S6:S36" si="2">SUMIFS(B6:P6,B$3:P$3,"AG")</f>
         <v>120.31</v>
       </c>
       <c r="T6" s="19">
-        <f>SUMIFS(B6:P6,B$3:P$3,"PB")</f>
+        <f t="shared" ref="T6:T36" si="3">SUMIFS(B6:P6,B$3:P$3,"PB")</f>
         <v>191.37</v>
       </c>
       <c r="U6" s="31">
-        <f t="shared" ref="U6:U37" si="0">Q6-(R6+S6+T6)</f>
+        <f t="shared" ref="U6:U37" si="4">Q6-(R6+S6+T6)</f>
         <v>0</v>
       </c>
     </row>
@@ -2230,34 +2230,32 @@
       <c r="F7" s="82"/>
       <c r="G7" s="82"/>
       <c r="H7" s="82"/>
-      <c r="I7" s="82">
-        <v>389.47</v>
-      </c>
+      <c r="I7" s="82"/>
       <c r="J7" s="82"/>
       <c r="K7" s="82"/>
       <c r="L7" s="82"/>
       <c r="M7" s="82"/>
       <c r="N7" s="82"/>
       <c r="O7" s="18"/>
-      <c r="P7" s="114"/>
+      <c r="P7" s="121"/>
       <c r="Q7" s="30">
-        <f>SUM(B7:P7)</f>
-        <v>450.73</v>
+        <f t="shared" si="0"/>
+        <v>61.26</v>
       </c>
       <c r="R7" s="19">
-        <f>SUMIFS(B7:P7,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S7" s="19">
-        <f>SUMIFS(B7:P7,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>61.26</v>
       </c>
       <c r="T7" s="19">
-        <f>SUMIFS(B7:P7,B$3:P$3,"PB")</f>
-        <v>389.47</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U7" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2274,34 +2272,32 @@
       <c r="F8" s="83"/>
       <c r="G8" s="83"/>
       <c r="H8" s="83"/>
-      <c r="I8" s="83">
-        <v>111.17</v>
-      </c>
+      <c r="I8" s="83"/>
       <c r="J8" s="83"/>
       <c r="K8" s="83"/>
       <c r="L8" s="83"/>
       <c r="M8" s="83"/>
       <c r="N8" s="83"/>
       <c r="O8" s="84"/>
-      <c r="P8" s="114"/>
+      <c r="P8" s="121"/>
       <c r="Q8" s="30">
-        <f>SUM(B8:P8)</f>
-        <v>257.7399999999999</v>
+        <f t="shared" si="0"/>
+        <v>146.56999999999991</v>
       </c>
       <c r="R8" s="19">
-        <f>SUMIFS(B8:P8,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S8" s="19">
-        <f>SUMIFS(B8:P8,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>146.56999999999991</v>
       </c>
       <c r="T8" s="19">
-        <f>SUMIFS(B8:P8,B$3:P$3,"PB")</f>
-        <v>111.17</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U8" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2323,25 +2319,25 @@
       <c r="M9" s="91"/>
       <c r="N9" s="91"/>
       <c r="O9" s="92"/>
-      <c r="P9" s="114"/>
+      <c r="P9" s="121"/>
       <c r="Q9" s="99">
-        <f>SUM(B9:P9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R9" s="100">
-        <f>SUMIFS(B9:P9,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S9" s="100">
-        <f>SUMIFS(B9:P9,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T9" s="100">
-        <f>SUMIFS(B9:P9,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U9" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2363,25 +2359,25 @@
       <c r="M10" s="61"/>
       <c r="N10" s="61"/>
       <c r="O10" s="59"/>
-      <c r="P10" s="114"/>
+      <c r="P10" s="121"/>
       <c r="Q10" s="99">
-        <f>SUM(B10:P10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R10" s="100">
-        <f>SUMIFS(B10:P10,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S10" s="100">
-        <f>SUMIFS(B10:P10,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T10" s="100">
-        <f>SUMIFS(B10:P10,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U10" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2407,25 +2403,25 @@
       <c r="M11" s="81"/>
       <c r="N11" s="81"/>
       <c r="O11" s="18"/>
-      <c r="P11" s="114"/>
+      <c r="P11" s="121"/>
       <c r="Q11" s="30">
-        <f>SUM(B11:P11)</f>
+        <f t="shared" si="0"/>
         <v>365.07000000000011</v>
       </c>
       <c r="R11" s="19">
-        <f>SUMIFS(B11:P11,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S11" s="19">
-        <f>SUMIFS(B11:P11,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>351.74000000000012</v>
       </c>
       <c r="T11" s="19">
-        <f>SUMIFS(B11:P11,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>13.33</v>
       </c>
       <c r="U11" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2453,25 +2449,25 @@
       <c r="M12" s="81"/>
       <c r="N12" s="81"/>
       <c r="O12" s="18"/>
-      <c r="P12" s="117"/>
+      <c r="P12" s="124"/>
       <c r="Q12" s="30">
-        <f>SUM(B12:P12)</f>
+        <f t="shared" si="0"/>
         <v>394.7</v>
       </c>
       <c r="R12" s="19">
-        <f>SUMIFS(B12:P12,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S12" s="19">
-        <f>SUMIFS(B12:P12,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>38.57</v>
       </c>
       <c r="T12" s="19">
-        <f>SUMIFS(B12:P12,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>356.13</v>
       </c>
       <c r="U12" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2499,25 +2495,25 @@
       <c r="M13" s="81"/>
       <c r="N13" s="81"/>
       <c r="O13" s="18"/>
-      <c r="P13" s="117"/>
+      <c r="P13" s="124"/>
       <c r="Q13" s="30">
-        <f>SUM(B13:P13)</f>
+        <f t="shared" si="0"/>
         <v>380.18</v>
       </c>
       <c r="R13" s="19">
-        <f>SUMIFS(B13:P13,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S13" s="19">
-        <f>SUMIFS(B13:P13,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>251.28</v>
       </c>
       <c r="T13" s="19">
-        <f>SUMIFS(B13:P13,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>128.9</v>
       </c>
       <c r="U13" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2543,25 +2539,25 @@
       <c r="M14" s="81"/>
       <c r="N14" s="81"/>
       <c r="O14" s="18"/>
-      <c r="P14" s="114"/>
+      <c r="P14" s="121"/>
       <c r="Q14" s="30">
-        <f>SUM(B14:P14)</f>
+        <f t="shared" si="0"/>
         <v>331.84000000000015</v>
       </c>
       <c r="R14" s="19">
-        <f>SUMIFS(B14:P14,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S14" s="19">
-        <f>SUMIFS(B14:P14,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>326.87000000000012</v>
       </c>
       <c r="T14" s="19">
-        <f>SUMIFS(B14:P14,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>4.97</v>
       </c>
       <c r="U14" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2587,25 +2583,25 @@
       <c r="M15" s="81"/>
       <c r="N15" s="81"/>
       <c r="O15" s="18"/>
-      <c r="P15" s="114"/>
+      <c r="P15" s="121"/>
       <c r="Q15" s="30">
-        <f>SUM(B15:P15)</f>
+        <f t="shared" si="0"/>
         <v>302.45999999999998</v>
       </c>
       <c r="R15" s="19">
-        <f>SUMIFS(B15:P15,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>163.41999999999999</v>
       </c>
       <c r="S15" s="19">
-        <f>SUMIFS(B15:P15,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>139.04</v>
       </c>
       <c r="T15" s="19">
-        <f>SUMIFS(B15:P15,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U15" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2627,25 +2623,25 @@
       <c r="M16" s="61"/>
       <c r="N16" s="61"/>
       <c r="O16" s="59"/>
-      <c r="P16" s="114"/>
+      <c r="P16" s="121"/>
       <c r="Q16" s="99">
-        <f>SUM(B16:P16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R16" s="100">
-        <f>SUMIFS(B16:P16,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S16" s="100">
-        <f>SUMIFS(B16:P16,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T16" s="100">
-        <f>SUMIFS(B16:P16,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U16" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2667,25 +2663,25 @@
       <c r="M17" s="61"/>
       <c r="N17" s="61"/>
       <c r="O17" s="59"/>
-      <c r="P17" s="114"/>
+      <c r="P17" s="121"/>
       <c r="Q17" s="99">
-        <f>SUM(B17:P17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R17" s="100">
-        <f>SUMIFS(B17:P17,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S17" s="100">
-        <f>SUMIFS(B17:P17,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T17" s="100">
-        <f>SUMIFS(B17:P17,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U17" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2711,25 +2707,25 @@
       <c r="M18" s="81"/>
       <c r="N18" s="81"/>
       <c r="O18" s="18"/>
-      <c r="P18" s="114"/>
+      <c r="P18" s="121"/>
       <c r="Q18" s="30">
-        <f>SUM(B18:P18)</f>
+        <f t="shared" si="0"/>
         <v>351.58000000000004</v>
       </c>
       <c r="R18" s="19">
-        <f>SUMIFS(B18:P18,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>231.27</v>
       </c>
       <c r="S18" s="19">
-        <f>SUMIFS(B18:P18,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>120.31</v>
       </c>
       <c r="T18" s="19">
-        <f>SUMIFS(B18:P18,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U18" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2755,25 +2751,25 @@
       <c r="M19" s="81"/>
       <c r="N19" s="81"/>
       <c r="O19" s="18"/>
-      <c r="P19" s="117"/>
+      <c r="P19" s="124"/>
       <c r="Q19" s="30">
-        <f>SUM(B19:P19)</f>
+        <f t="shared" si="0"/>
         <v>134.82999999999998</v>
       </c>
       <c r="R19" s="19">
-        <f>SUMIFS(B19:P19,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S19" s="19">
-        <f>SUMIFS(B19:P19,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>61.26</v>
       </c>
       <c r="T19" s="19">
-        <f>SUMIFS(B19:P19,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>73.569999999999993</v>
       </c>
       <c r="U19" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2799,25 +2795,25 @@
       <c r="M20" s="81"/>
       <c r="N20" s="81"/>
       <c r="O20" s="18"/>
-      <c r="P20" s="117"/>
+      <c r="P20" s="124"/>
       <c r="Q20" s="30">
-        <f>SUM(B20:P20)</f>
+        <f t="shared" si="0"/>
         <v>213.35</v>
       </c>
       <c r="R20" s="19">
-        <f>SUMIFS(B20:P20,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S20" s="19">
-        <f>SUMIFS(B20:P20,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>89.509999999999991</v>
       </c>
       <c r="T20" s="19">
-        <f>SUMIFS(B20:P20,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>123.84</v>
       </c>
       <c r="U20" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2843,25 +2839,25 @@
       </c>
       <c r="N21" s="81"/>
       <c r="O21" s="18"/>
-      <c r="P21" s="114"/>
+      <c r="P21" s="121"/>
       <c r="Q21" s="30">
-        <f>SUM(B21:P21)</f>
+        <f t="shared" si="0"/>
         <v>89.67</v>
       </c>
       <c r="R21" s="19">
-        <f>SUMIFS(B21:P21,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S21" s="19">
-        <f>SUMIFS(B21:P21,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>89.67</v>
       </c>
       <c r="T21" s="19">
-        <f>SUMIFS(B21:P21,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U21" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2883,25 +2879,25 @@
       <c r="M22" s="81"/>
       <c r="N22" s="81"/>
       <c r="O22" s="18"/>
-      <c r="P22" s="114"/>
+      <c r="P22" s="121"/>
       <c r="Q22" s="30">
-        <f>SUM(B22:P22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R22" s="19">
-        <f>SUMIFS(B22:P22,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S22" s="19">
-        <f>SUMIFS(B22:P22,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T22" s="19">
-        <f>SUMIFS(B22:P22,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U22" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2923,25 +2919,25 @@
       <c r="M23" s="61"/>
       <c r="N23" s="61"/>
       <c r="O23" s="59"/>
-      <c r="P23" s="114"/>
+      <c r="P23" s="121"/>
       <c r="Q23" s="99">
-        <f>SUM(B23:P23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R23" s="100">
-        <f>SUMIFS(B23:P23,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S23" s="100">
-        <f>SUMIFS(B23:P23,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T23" s="100">
-        <f>SUMIFS(B23:P23,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U23" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2963,25 +2959,25 @@
       <c r="M24" s="61"/>
       <c r="N24" s="61"/>
       <c r="O24" s="59"/>
-      <c r="P24" s="114"/>
+      <c r="P24" s="121"/>
       <c r="Q24" s="99">
-        <f>SUM(B24:P24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R24" s="100">
-        <f>SUMIFS(B24:P24,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S24" s="100">
-        <f>SUMIFS(B24:P24,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T24" s="100">
-        <f>SUMIFS(B24:P24,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U24" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3003,25 +2999,25 @@
       <c r="M25" s="81"/>
       <c r="N25" s="81"/>
       <c r="O25" s="18"/>
-      <c r="P25" s="114"/>
+      <c r="P25" s="121"/>
       <c r="Q25" s="30">
-        <f>SUM(B25:P25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R25" s="19">
-        <f>SUMIFS(B25:P25,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S25" s="19">
-        <f>SUMIFS(B25:P25,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T25" s="19">
-        <f>SUMIFS(B25:P25,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U25" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3043,25 +3039,25 @@
       <c r="M26" s="81"/>
       <c r="N26" s="81"/>
       <c r="O26" s="18"/>
-      <c r="P26" s="117"/>
+      <c r="P26" s="124"/>
       <c r="Q26" s="30">
-        <f>SUM(B26:P26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R26" s="19">
-        <f>SUMIFS(B26:P26,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S26" s="19">
-        <f>SUMIFS(B26:P26,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T26" s="19">
-        <f>SUMIFS(B26:P26,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U26" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3083,25 +3079,25 @@
       <c r="M27" s="81"/>
       <c r="N27" s="81"/>
       <c r="O27" s="18"/>
-      <c r="P27" s="117"/>
+      <c r="P27" s="124"/>
       <c r="Q27" s="30">
-        <f>SUM(B27:P27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R27" s="19">
-        <f>SUMIFS(B27:P27,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S27" s="19">
-        <f>SUMIFS(B27:P27,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T27" s="19">
-        <f>SUMIFS(B27:P27,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U27" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3123,25 +3119,25 @@
       <c r="M28" s="81"/>
       <c r="N28" s="81"/>
       <c r="O28" s="18"/>
-      <c r="P28" s="114"/>
+      <c r="P28" s="121"/>
       <c r="Q28" s="30">
-        <f>SUM(B28:P28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R28" s="19">
-        <f>SUMIFS(B28:P28,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S28" s="19">
-        <f>SUMIFS(B28:P28,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T28" s="19">
-        <f>SUMIFS(B28:P28,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U28" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3163,25 +3159,25 @@
       <c r="M29" s="81"/>
       <c r="N29" s="81"/>
       <c r="O29" s="18"/>
-      <c r="P29" s="118"/>
+      <c r="P29" s="125"/>
       <c r="Q29" s="30">
-        <f>SUM(B29:P29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R29" s="19">
-        <f>SUMIFS(B29:P29,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S29" s="19">
-        <f>SUMIFS(B29:P29,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T29" s="19">
-        <f>SUMIFS(B29:P29,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U29" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3203,25 +3199,25 @@
       <c r="M30" s="61"/>
       <c r="N30" s="61"/>
       <c r="O30" s="59"/>
-      <c r="P30" s="118"/>
+      <c r="P30" s="125"/>
       <c r="Q30" s="99">
-        <f>SUM(B30:P30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R30" s="100">
-        <f>SUMIFS(B30:P30,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S30" s="100">
-        <f>SUMIFS(B30:P30,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T30" s="100">
-        <f>SUMIFS(B30:P30,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U30" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3243,25 +3239,25 @@
       <c r="M31" s="61"/>
       <c r="N31" s="61"/>
       <c r="O31" s="59"/>
-      <c r="P31" s="118"/>
+      <c r="P31" s="125"/>
       <c r="Q31" s="99">
-        <f>SUM(B31:P31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R31" s="100">
-        <f>SUMIFS(B31:P31,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S31" s="100">
-        <f>SUMIFS(B31:P31,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T31" s="100">
-        <f>SUMIFS(B31:P31,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U31" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3283,25 +3279,25 @@
       <c r="M32" s="81"/>
       <c r="N32" s="81"/>
       <c r="O32" s="18"/>
-      <c r="P32" s="118"/>
+      <c r="P32" s="125"/>
       <c r="Q32" s="30">
-        <f>SUM(B32:P32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R32" s="19">
-        <f>SUMIFS(B32:P32,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S32" s="19">
-        <f>SUMIFS(B32:P32,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T32" s="19">
-        <f>SUMIFS(B32:P32,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U32" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3323,25 +3319,25 @@
       <c r="M33" s="81"/>
       <c r="N33" s="81"/>
       <c r="O33" s="18"/>
-      <c r="P33" s="118"/>
+      <c r="P33" s="125"/>
       <c r="Q33" s="30">
-        <f>SUM(B33:P33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R33" s="19">
-        <f>SUMIFS(B33:P33,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S33" s="19">
-        <f>SUMIFS(B33:P33,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T33" s="19">
-        <f>SUMIFS(B33:P33,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U33" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3363,25 +3359,25 @@
       <c r="M34" s="81"/>
       <c r="N34" s="81"/>
       <c r="O34" s="18"/>
-      <c r="P34" s="118"/>
+      <c r="P34" s="125"/>
       <c r="Q34" s="30">
-        <f>SUM(B34:P34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R34" s="19">
-        <f>SUMIFS(B34:P34,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S34" s="19">
-        <f>SUMIFS(B34:P34,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T34" s="19">
-        <f>SUMIFS(B34:P34,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U34" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3403,25 +3399,25 @@
       <c r="M35" s="81"/>
       <c r="N35" s="81"/>
       <c r="O35" s="18"/>
-      <c r="P35" s="118"/>
+      <c r="P35" s="125"/>
       <c r="Q35" s="30">
-        <f>SUM(B35:P35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R35" s="19">
-        <f>SUMIFS(B35:P35,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S35" s="19">
-        <f>SUMIFS(B35:P35,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T35" s="19">
-        <f>SUMIFS(B35:P35,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U35" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3443,25 +3439,25 @@
       <c r="M36" s="81"/>
       <c r="N36" s="81"/>
       <c r="O36" s="18"/>
-      <c r="P36" s="118"/>
+      <c r="P36" s="125"/>
       <c r="Q36" s="30">
-        <f>SUM(B36:P36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R36" s="19">
-        <f>SUMIFS(B36:P36,B$3:P$3,"WB")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S36" s="19">
-        <f>SUMIFS(B36:P36,B$3:P$3,"AG")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T36" s="19">
-        <f>SUMIFS(B36:P36,B$3:P$3,"PB")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U36" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3470,23 +3466,23 @@
         <v>32</v>
       </c>
       <c r="B37" s="21">
-        <f t="shared" ref="B37:F37" si="1">SUM(B6:B36)</f>
+        <f t="shared" ref="B37:F37" si="5">SUM(B6:B36)</f>
         <v>191.37</v>
       </c>
       <c r="C37" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>718.45</v>
       </c>
       <c r="D37" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>470.38</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>27.98</v>
       </c>
       <c r="F37" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>717.19</v>
       </c>
       <c r="G37" s="21"/>
@@ -3501,7 +3497,7 @@
       <c r="P37" s="35"/>
       <c r="Q37" s="33">
         <f>SUM(Q6:Q36)</f>
-        <v>3583.83</v>
+        <v>3083.19</v>
       </c>
       <c r="R37" s="28">
         <f>SUM(R6:R36)</f>
@@ -3513,10 +3509,10 @@
       </c>
       <c r="T37" s="28">
         <f>SUM(T6:T36)</f>
-        <v>1392.75</v>
+        <v>892.11</v>
       </c>
       <c r="U37" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD37" s="1"/>
@@ -3644,7 +3640,7 @@
       <c r="P38" s="36"/>
       <c r="Q38" s="34">
         <f>P37-Q37</f>
-        <v>-3583.83</v>
+        <v>-3083.19</v>
       </c>
     </row>
     <row r="39" spans="1:126" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3744,51 +3740,51 @@
         <v>36</v>
       </c>
       <c r="B41" s="64">
-        <f t="shared" ref="B41:M41" si="2">B40-B37</f>
+        <f t="shared" ref="B41:M41" si="6">B40-B37</f>
         <v>0</v>
       </c>
       <c r="C41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.97</v>
       </c>
       <c r="H41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>394.69</v>
       </c>
       <c r="I41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>500.64</v>
       </c>
       <c r="J41" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>197.41</v>
       </c>
       <c r="K41" s="74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>763.87999999999943</v>
       </c>
       <c r="L41" s="74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>417.31</v>
       </c>
       <c r="M41" s="74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8.1999999999999993</v>
       </c>
       <c r="N41" s="74"/>
@@ -3832,16 +3828,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="U1:U5"/>
+    <mergeCell ref="P1:P36"/>
+    <mergeCell ref="S1:S5"/>
+    <mergeCell ref="R1:R5"/>
+    <mergeCell ref="Q1:Q5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="T1:T5"/>
-    <mergeCell ref="U1:U5"/>
-    <mergeCell ref="P1:P36"/>
-    <mergeCell ref="S1:S5"/>
-    <mergeCell ref="R1:R5"/>
-    <mergeCell ref="Q1:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="84" fitToWidth="0" orientation="landscape"/>
@@ -3855,7 +3851,7 @@
   </sheetPr>
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -3883,53 +3879,53 @@
       <c r="D1" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="127" t="s">
+      <c r="E1" s="131" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="128"/>
-      <c r="G1" s="129" t="s">
+      <c r="F1" s="132"/>
+      <c r="G1" s="133" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="128"/>
+      <c r="H1" s="132"/>
       <c r="I1" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="129" t="s">
+      <c r="J1" s="133" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="128"/>
+      <c r="K1" s="132"/>
       <c r="L1" s="57"/>
-      <c r="M1" s="130" t="s">
+      <c r="M1" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="120" t="s">
+      <c r="N1" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="120" t="s">
+      <c r="O1" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="120" t="s">
+      <c r="P1" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="120" t="s">
+      <c r="Q1" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="120" t="s">
+      <c r="R1" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="120" t="s">
+      <c r="S1" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="119" t="s">
+      <c r="T1" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="119" t="s">
+      <c r="U1" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="119" t="s">
+      <c r="V1" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="110" t="s">
+      <c r="W1" s="119" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3968,17 +3964,17 @@
         <v>1</v>
       </c>
       <c r="L2" s="109"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -4015,17 +4011,17 @@
         <v>24</v>
       </c>
       <c r="L3" s="109"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="111"/>
-      <c r="O3" s="111"/>
-      <c r="P3" s="111"/>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="111"/>
-      <c r="S3" s="111"/>
-      <c r="T3" s="111"/>
-      <c r="U3" s="111"/>
-      <c r="V3" s="111"/>
-      <c r="W3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
     </row>
     <row r="4" spans="1:23" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
@@ -4040,33 +4036,33 @@
       <c r="D4" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="134" t="s">
+      <c r="E4" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="124"/>
-      <c r="G4" s="123" t="s">
+      <c r="F4" s="113"/>
+      <c r="G4" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="124"/>
+      <c r="H4" s="113"/>
       <c r="I4" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="123" t="s">
+      <c r="J4" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="124"/>
+      <c r="K4" s="113"/>
       <c r="L4" s="57"/>
-      <c r="M4" s="122"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="111"/>
+      <c r="M4" s="111"/>
+      <c r="N4" s="117"/>
+      <c r="O4" s="117"/>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="117"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
+      <c r="T4" s="117"/>
+      <c r="U4" s="117"/>
+      <c r="V4" s="117"/>
+      <c r="W4" s="117"/>
     </row>
     <row r="5" spans="1:23" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88" t="s">
@@ -4093,17 +4089,17 @@
         <v>55</v>
       </c>
       <c r="L5" s="87"/>
-      <c r="M5" s="122"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="112"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
     </row>
     <row r="6" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="93">
@@ -4122,45 +4118,45 @@
       <c r="J6" s="85"/>
       <c r="K6" s="85"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="122"/>
+      <c r="M6" s="111"/>
       <c r="N6" s="19">
-        <f>SUMIFS(B6:M6,B$2:M$2,"DW")</f>
+        <f t="shared" ref="N6:N36" si="0">SUMIFS(B6:M6,B$2:M$2,"DW")</f>
         <v>105.77</v>
       </c>
       <c r="O6" s="19">
-        <f>SUMIFS(B6:M6,B$2:M$2,"TW")</f>
+        <f t="shared" ref="O6:O36" si="1">SUMIFS(B6:M6,B$2:M$2,"TW")</f>
         <v>0</v>
       </c>
       <c r="P6" s="19">
-        <f>SUMIFS(B6:M6,B$2:M$2,"SW")</f>
+        <f t="shared" ref="P6:P36" si="2">SUMIFS(B6:M6,B$2:M$2,"SW")</f>
         <v>0</v>
       </c>
       <c r="Q6" s="19">
-        <f>SUMIFS(B6:M6,B$2:M$2,"f")</f>
+        <f t="shared" ref="Q6:Q36" si="3">SUMIFS(B6:M6,B$2:M$2,"f")</f>
         <v>0</v>
       </c>
       <c r="R6" s="19">
-        <f>SUMIFS(B6:M6,B$2:M$2,"B")</f>
+        <f t="shared" ref="R6:R36" si="4">SUMIFS(B6:M6,B$2:M$2,"B")</f>
         <v>0</v>
       </c>
       <c r="S6" s="19">
-        <f>SUMIFS(B6:M6,B$2:M$2,"S")</f>
+        <f t="shared" ref="S6:S36" si="5">SUMIFS(B6:M6,B$2:M$2,"S")</f>
         <v>0</v>
       </c>
       <c r="T6" s="19">
-        <f>SUMIFS(B6:M6,B$3:M$3,"WB")</f>
+        <f t="shared" ref="T6:T36" si="6">SUMIFS(B6:M6,B$3:M$3,"WB")</f>
         <v>0</v>
       </c>
       <c r="U6" s="19">
-        <f>SUMIFS(B6:M6,B$3:M$3,"AG")</f>
+        <f t="shared" ref="U6:U36" si="7">SUMIFS(B6:M6,B$3:M$3,"AG")</f>
         <v>105.77</v>
       </c>
       <c r="V6" s="19">
-        <f>SUMIFS(B6:M6,B$3:M$3,"PB")</f>
+        <f t="shared" ref="V6:V36" si="8">SUMIFS(B6:M6,B$3:M$3,"PB")</f>
         <v>0</v>
       </c>
       <c r="W6" s="31">
-        <f t="shared" ref="W6:W37" si="0">N6+O6+P6+Q6+R6+S6-(T6+U6+V6)</f>
+        <f t="shared" ref="W6:W37" si="9">N6+O6+P6+Q6+R6+S6-(T6+U6+V6)</f>
         <v>0</v>
       </c>
     </row>
@@ -4181,45 +4177,45 @@
       <c r="J7" s="82"/>
       <c r="K7" s="82"/>
       <c r="L7" s="18"/>
-      <c r="M7" s="122"/>
+      <c r="M7" s="111"/>
       <c r="N7" s="19">
-        <f>SUMIFS(B7:M7,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>157.43</v>
       </c>
       <c r="O7" s="19">
-        <f>SUMIFS(B7:M7,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7" s="19">
-        <f>SUMIFS(B7:M7,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q7" s="19">
-        <f>SUMIFS(B7:M7,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R7" s="19">
-        <f>SUMIFS(B7:M7,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S7" s="19">
-        <f>SUMIFS(B7:M7,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T7" s="19">
-        <f>SUMIFS(B7:M7,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U7" s="19">
-        <f>SUMIFS(B7:M7,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>157.43</v>
       </c>
       <c r="V7" s="19">
-        <f>SUMIFS(B7:M7,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W7" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4242,45 +4238,45 @@
       <c r="J8" s="83"/>
       <c r="K8" s="83"/>
       <c r="L8" s="84"/>
-      <c r="M8" s="122"/>
+      <c r="M8" s="111"/>
       <c r="N8" s="19">
-        <f>SUMIFS(B8:M8,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>64.19</v>
       </c>
       <c r="O8" s="19">
-        <f>SUMIFS(B8:M8,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>28.96</v>
       </c>
       <c r="P8" s="19">
-        <f>SUMIFS(B8:M8,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q8" s="19">
-        <f>SUMIFS(B8:M8,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R8" s="19">
-        <f>SUMIFS(B8:M8,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S8" s="19">
-        <f>SUMIFS(B8:M8,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T8" s="19">
-        <f>SUMIFS(B8:M8,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U8" s="19">
-        <f>SUMIFS(B8:M8,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>93.15</v>
       </c>
       <c r="V8" s="19">
-        <f>SUMIFS(B8:M8,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W8" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4303,45 +4299,45 @@
       <c r="J9" s="91"/>
       <c r="K9" s="91"/>
       <c r="L9" s="92"/>
-      <c r="M9" s="122"/>
+      <c r="M9" s="111"/>
       <c r="N9" s="60">
-        <f>SUMIFS(B9:M9,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>84.1</v>
       </c>
       <c r="O9" s="60">
-        <f>SUMIFS(B9:M9,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>29.12</v>
       </c>
       <c r="P9" s="60">
-        <f>SUMIFS(B9:M9,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q9" s="60">
-        <f>SUMIFS(B9:M9,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R9" s="60">
-        <f>SUMIFS(B9:M9,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S9" s="60">
-        <f>SUMIFS(B9:M9,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T9" s="60">
-        <f>SUMIFS(B9:M9,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U9" s="60">
-        <f>SUMIFS(B9:M9,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>113.22</v>
       </c>
       <c r="V9" s="60">
-        <f>SUMIFS(B9:M9,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W9" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4360,45 +4356,45 @@
       <c r="J10" s="61"/>
       <c r="K10" s="61"/>
       <c r="L10" s="59"/>
-      <c r="M10" s="122"/>
+      <c r="M10" s="111"/>
       <c r="N10" s="60">
-        <f>SUMIFS(B10:M10,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O10" s="60">
-        <f>SUMIFS(B10:M10,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P10" s="60">
-        <f>SUMIFS(B10:M10,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q10" s="60">
-        <f>SUMIFS(B10:M10,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R10" s="60">
-        <f>SUMIFS(B10:M10,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S10" s="60">
-        <f>SUMIFS(B10:M10,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T10" s="60">
-        <f>SUMIFS(B10:M10,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U10" s="60">
-        <f>SUMIFS(B10:M10,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V10" s="60">
-        <f>SUMIFS(B10:M10,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W10" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4421,45 +4417,45 @@
       <c r="J11" s="81"/>
       <c r="K11" s="81"/>
       <c r="L11" s="18"/>
-      <c r="M11" s="122"/>
+      <c r="M11" s="111"/>
       <c r="N11" s="19">
-        <f>SUMIFS(B11:M11,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>60.14</v>
       </c>
       <c r="O11" s="19">
-        <f>SUMIFS(B11:M11,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>46.89</v>
       </c>
       <c r="P11" s="19">
-        <f>SUMIFS(B11:M11,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q11" s="19">
-        <f>SUMIFS(B11:M11,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R11" s="19">
-        <f>SUMIFS(B11:M11,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S11" s="19">
-        <f>SUMIFS(B11:M11,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T11" s="19">
-        <f>SUMIFS(B11:M11,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U11" s="19">
-        <f>SUMIFS(B11:M11,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>107.03</v>
       </c>
       <c r="V11" s="19">
-        <f>SUMIFS(B11:M11,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W11" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4480,45 +4476,45 @@
       <c r="J12" s="81"/>
       <c r="K12" s="81"/>
       <c r="L12" s="18"/>
-      <c r="M12" s="122"/>
+      <c r="M12" s="111"/>
       <c r="N12" s="19">
-        <f>SUMIFS(B12:M12,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>107.95</v>
       </c>
       <c r="O12" s="19">
-        <f>SUMIFS(B12:M12,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P12" s="19">
-        <f>SUMIFS(B12:M12,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q12" s="19">
-        <f>SUMIFS(B12:M12,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R12" s="19">
-        <f>SUMIFS(B12:M12,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S12" s="19">
-        <f>SUMIFS(B12:M12,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T12" s="19">
-        <f>SUMIFS(B12:M12,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U12" s="19">
-        <f>SUMIFS(B12:M12,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>107.95</v>
       </c>
       <c r="V12" s="19">
-        <f>SUMIFS(B12:M12,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W12" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4539,45 +4535,45 @@
       <c r="J13" s="81"/>
       <c r="K13" s="81"/>
       <c r="L13" s="18"/>
-      <c r="M13" s="122"/>
+      <c r="M13" s="111"/>
       <c r="N13" s="19">
-        <f>SUMIFS(B13:M13,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>135.21</v>
       </c>
       <c r="O13" s="19">
-        <f>SUMIFS(B13:M13,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P13" s="19">
-        <f>SUMIFS(B13:M13,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q13" s="19">
-        <f>SUMIFS(B13:M13,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R13" s="19">
-        <f>SUMIFS(B13:M13,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S13" s="19">
-        <f>SUMIFS(B13:M13,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T13" s="19">
-        <f>SUMIFS(B13:M13,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U13" s="19">
-        <f>SUMIFS(B13:M13,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>135.21</v>
       </c>
       <c r="V13" s="19">
-        <f>SUMIFS(B13:M13,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W13" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4598,45 +4594,45 @@
       <c r="J14" s="81"/>
       <c r="K14" s="81"/>
       <c r="L14" s="18"/>
-      <c r="M14" s="122"/>
+      <c r="M14" s="111"/>
       <c r="N14" s="19">
-        <f>SUMIFS(B14:M14,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>113.81</v>
       </c>
       <c r="O14" s="19">
-        <f>SUMIFS(B14:M14,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P14" s="19">
-        <f>SUMIFS(B14:M14,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q14" s="19">
-        <f>SUMIFS(B14:M14,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14" s="19">
-        <f>SUMIFS(B14:M14,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S14" s="19">
-        <f>SUMIFS(B14:M14,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T14" s="19">
-        <f>SUMIFS(B14:M14,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U14" s="19">
-        <f>SUMIFS(B14:M14,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>113.81</v>
       </c>
       <c r="V14" s="19">
-        <f>SUMIFS(B14:M14,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W14" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4657,45 +4653,45 @@
       <c r="J15" s="81"/>
       <c r="K15" s="81"/>
       <c r="L15" s="18"/>
-      <c r="M15" s="122"/>
+      <c r="M15" s="111"/>
       <c r="N15" s="19">
-        <f>SUMIFS(B15:M15,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>67.36999999999999</v>
       </c>
       <c r="O15" s="19">
-        <f>SUMIFS(B15:M15,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P15" s="19">
-        <f>SUMIFS(B15:M15,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q15" s="19">
-        <f>SUMIFS(B15:M15,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R15" s="19">
-        <f>SUMIFS(B15:M15,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S15" s="19">
-        <f>SUMIFS(B15:M15,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T15" s="19">
-        <f>SUMIFS(B15:M15,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U15" s="19">
-        <f>SUMIFS(B15:M15,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>67.36999999999999</v>
       </c>
       <c r="V15" s="19">
-        <f>SUMIFS(B15:M15,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W15" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4716,45 +4712,45 @@
       <c r="J16" s="61"/>
       <c r="K16" s="61"/>
       <c r="L16" s="59"/>
-      <c r="M16" s="122"/>
+      <c r="M16" s="111"/>
       <c r="N16" s="60">
-        <f>SUMIFS(B16:M16,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>80.63</v>
       </c>
       <c r="O16" s="60">
-        <f>SUMIFS(B16:M16,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" s="60">
-        <f>SUMIFS(B16:M16,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q16" s="60">
-        <f>SUMIFS(B16:M16,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R16" s="60">
-        <f>SUMIFS(B16:M16,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S16" s="60">
-        <f>SUMIFS(B16:M16,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T16" s="60">
-        <f>SUMIFS(B16:M16,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U16" s="60">
-        <f>SUMIFS(B16:M16,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>80.63</v>
       </c>
       <c r="V16" s="60">
-        <f>SUMIFS(B16:M16,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W16" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4773,45 +4769,45 @@
       <c r="J17" s="61"/>
       <c r="K17" s="61"/>
       <c r="L17" s="59"/>
-      <c r="M17" s="122"/>
+      <c r="M17" s="111"/>
       <c r="N17" s="60">
-        <f>SUMIFS(B17:M17,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O17" s="60">
-        <f>SUMIFS(B17:M17,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P17" s="60">
-        <f>SUMIFS(B17:M17,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q17" s="60">
-        <f>SUMIFS(B17:M17,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R17" s="60">
-        <f>SUMIFS(B17:M17,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S17" s="60">
-        <f>SUMIFS(B17:M17,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T17" s="60">
-        <f>SUMIFS(B17:M17,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U17" s="60">
-        <f>SUMIFS(B17:M17,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V17" s="60">
-        <f>SUMIFS(B17:M17,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W17" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4836,45 +4832,45 @@
       <c r="J18" s="81"/>
       <c r="K18" s="81"/>
       <c r="L18" s="18"/>
-      <c r="M18" s="122"/>
+      <c r="M18" s="111"/>
       <c r="N18" s="19">
-        <f>SUMIFS(B18:M18,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>114.8</v>
       </c>
       <c r="O18" s="19">
-        <f>SUMIFS(B18:M18,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>23.41</v>
       </c>
       <c r="P18" s="19">
-        <f>SUMIFS(B18:M18,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q18" s="19">
-        <f>SUMIFS(B18:M18,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R18" s="19">
-        <f>SUMIFS(B18:M18,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S18" s="19">
-        <f>SUMIFS(B18:M18,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T18" s="19">
-        <f>SUMIFS(B18:M18,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U18" s="19">
-        <f>SUMIFS(B18:M18,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>138.21</v>
       </c>
       <c r="V18" s="19">
-        <f>SUMIFS(B18:M18,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W18" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4897,45 +4893,45 @@
       <c r="J19" s="81"/>
       <c r="K19" s="81"/>
       <c r="L19" s="18"/>
-      <c r="M19" s="122"/>
+      <c r="M19" s="111"/>
       <c r="N19" s="19">
-        <f>SUMIFS(B19:M19,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>79.77</v>
       </c>
       <c r="O19" s="19">
-        <f>SUMIFS(B19:M19,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>60.56</v>
       </c>
       <c r="P19" s="19">
-        <f>SUMIFS(B19:M19,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q19" s="19">
-        <f>SUMIFS(B19:M19,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R19" s="19">
-        <f>SUMIFS(B19:M19,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S19" s="19">
-        <f>SUMIFS(B19:M19,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T19" s="19">
-        <f>SUMIFS(B19:M19,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U19" s="19">
-        <f>SUMIFS(B19:M19,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>140.32999999999998</v>
       </c>
       <c r="V19" s="19">
-        <f>SUMIFS(B19:M19,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W19" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4962,45 +4958,45 @@
       <c r="J20" s="81"/>
       <c r="K20" s="81"/>
       <c r="L20" s="18"/>
-      <c r="M20" s="122"/>
+      <c r="M20" s="111"/>
       <c r="N20" s="19">
-        <f>SUMIFS(B20:M20,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>87.84</v>
       </c>
       <c r="O20" s="19">
-        <f>SUMIFS(B20:M20,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>52.91</v>
       </c>
       <c r="P20" s="19">
-        <f>SUMIFS(B20:M20,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q20" s="19">
-        <f>SUMIFS(B20:M20,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R20" s="19">
-        <f>SUMIFS(B20:M20,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S20" s="19">
-        <f>SUMIFS(B20:M20,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T20" s="19">
-        <f>SUMIFS(B20:M20,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U20" s="19">
-        <f>SUMIFS(B20:M20,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>140.75</v>
       </c>
       <c r="V20" s="19">
-        <f>SUMIFS(B20:M20,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W20" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5029,45 +5025,45 @@
       <c r="J21" s="81"/>
       <c r="K21" s="81"/>
       <c r="L21" s="18"/>
-      <c r="M21" s="122"/>
+      <c r="M21" s="111"/>
       <c r="N21" s="19">
-        <f>SUMIFS(B21:M21,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>155.69</v>
       </c>
       <c r="O21" s="19">
-        <f>SUMIFS(B21:M21,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>29.84</v>
       </c>
       <c r="P21" s="19">
-        <f>SUMIFS(B21:M21,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q21" s="19">
-        <f>SUMIFS(B21:M21,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R21" s="19">
-        <f>SUMIFS(B21:M21,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S21" s="19">
-        <f>SUMIFS(B21:M21,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T21" s="19">
-        <f>SUMIFS(B21:M21,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U21" s="19">
-        <f>SUMIFS(B21:M21,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>159.20000000000002</v>
       </c>
       <c r="V21" s="19">
-        <f>SUMIFS(B21:M21,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>26.33</v>
       </c>
       <c r="W21" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5086,45 +5082,45 @@
       <c r="J22" s="81"/>
       <c r="K22" s="81"/>
       <c r="L22" s="18"/>
-      <c r="M22" s="122"/>
+      <c r="M22" s="111"/>
       <c r="N22" s="19">
-        <f>SUMIFS(B22:M22,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O22" s="19">
-        <f>SUMIFS(B22:M22,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P22" s="19">
-        <f>SUMIFS(B22:M22,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q22" s="19">
-        <f>SUMIFS(B22:M22,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R22" s="19">
-        <f>SUMIFS(B22:M22,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S22" s="19">
-        <f>SUMIFS(B22:M22,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T22" s="19">
-        <f>SUMIFS(B22:M22,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U22" s="19">
-        <f>SUMIFS(B22:M22,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V22" s="19">
-        <f>SUMIFS(B22:M22,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W22" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5143,45 +5139,45 @@
       <c r="J23" s="61"/>
       <c r="K23" s="61"/>
       <c r="L23" s="59"/>
-      <c r="M23" s="122"/>
+      <c r="M23" s="111"/>
       <c r="N23" s="60">
-        <f>SUMIFS(B23:M23,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O23" s="60">
-        <f>SUMIFS(B23:M23,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P23" s="60">
-        <f>SUMIFS(B23:M23,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q23" s="60">
-        <f>SUMIFS(B23:M23,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R23" s="60">
-        <f>SUMIFS(B23:M23,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S23" s="60">
-        <f>SUMIFS(B23:M23,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T23" s="60">
-        <f>SUMIFS(B23:M23,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U23" s="60">
-        <f>SUMIFS(B23:M23,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V23" s="60">
-        <f>SUMIFS(B23:M23,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W23" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5200,45 +5196,45 @@
       <c r="J24" s="61"/>
       <c r="K24" s="61"/>
       <c r="L24" s="59"/>
-      <c r="M24" s="122"/>
+      <c r="M24" s="111"/>
       <c r="N24" s="60">
-        <f>SUMIFS(B24:M24,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O24" s="60">
-        <f>SUMIFS(B24:M24,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P24" s="60">
-        <f>SUMIFS(B24:M24,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q24" s="60">
-        <f>SUMIFS(B24:M24,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R24" s="60">
-        <f>SUMIFS(B24:M24,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S24" s="60">
-        <f>SUMIFS(B24:M24,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T24" s="60">
-        <f>SUMIFS(B24:M24,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U24" s="60">
-        <f>SUMIFS(B24:M24,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V24" s="60">
-        <f>SUMIFS(B24:M24,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W24" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5257,45 +5253,45 @@
       <c r="J25" s="81"/>
       <c r="K25" s="81"/>
       <c r="L25" s="18"/>
-      <c r="M25" s="122"/>
+      <c r="M25" s="111"/>
       <c r="N25" s="19">
-        <f>SUMIFS(B25:M25,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O25" s="19">
-        <f>SUMIFS(B25:M25,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P25" s="19">
-        <f>SUMIFS(B25:M25,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q25" s="19">
-        <f>SUMIFS(B25:M25,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R25" s="19">
-        <f>SUMIFS(B25:M25,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S25" s="19">
-        <f>SUMIFS(B25:M25,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T25" s="19">
-        <f>SUMIFS(B25:M25,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U25" s="19">
-        <f>SUMIFS(B25:M25,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V25" s="19">
-        <f>SUMIFS(B25:M25,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W25" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5314,45 +5310,45 @@
       <c r="J26" s="81"/>
       <c r="K26" s="81"/>
       <c r="L26" s="18"/>
-      <c r="M26" s="122"/>
+      <c r="M26" s="111"/>
       <c r="N26" s="19">
-        <f>SUMIFS(B26:M26,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O26" s="19">
-        <f>SUMIFS(B26:M26,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P26" s="19">
-        <f>SUMIFS(B26:M26,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q26" s="19">
-        <f>SUMIFS(B26:M26,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R26" s="19">
-        <f>SUMIFS(B26:M26,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S26" s="19">
-        <f>SUMIFS(B26:M26,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T26" s="19">
-        <f>SUMIFS(B26:M26,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U26" s="19">
-        <f>SUMIFS(B26:M26,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V26" s="19">
-        <f>SUMIFS(B26:M26,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W26" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5371,45 +5367,45 @@
       <c r="J27" s="81"/>
       <c r="K27" s="81"/>
       <c r="L27" s="18"/>
-      <c r="M27" s="122"/>
+      <c r="M27" s="111"/>
       <c r="N27" s="19">
-        <f>SUMIFS(B27:M27,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O27" s="19">
-        <f>SUMIFS(B27:M27,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P27" s="19">
-        <f>SUMIFS(B27:M27,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q27" s="19">
-        <f>SUMIFS(B27:M27,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R27" s="19">
-        <f>SUMIFS(B27:M27,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S27" s="19">
-        <f>SUMIFS(B27:M27,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T27" s="19">
-        <f>SUMIFS(B27:M27,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U27" s="19">
-        <f>SUMIFS(B27:M27,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V27" s="19">
-        <f>SUMIFS(B27:M27,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W27" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5428,45 +5424,45 @@
       <c r="J28" s="81"/>
       <c r="K28" s="81"/>
       <c r="L28" s="18"/>
-      <c r="M28" s="122"/>
+      <c r="M28" s="111"/>
       <c r="N28" s="19">
-        <f>SUMIFS(B28:M28,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O28" s="19">
-        <f>SUMIFS(B28:M28,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P28" s="19">
-        <f>SUMIFS(B28:M28,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q28" s="19">
-        <f>SUMIFS(B28:M28,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R28" s="19">
-        <f>SUMIFS(B28:M28,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S28" s="19">
-        <f>SUMIFS(B28:M28,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T28" s="19">
-        <f>SUMIFS(B28:M28,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U28" s="19">
-        <f>SUMIFS(B28:M28,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V28" s="19">
-        <f>SUMIFS(B28:M28,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W28" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5485,45 +5481,45 @@
       <c r="J29" s="81"/>
       <c r="K29" s="81"/>
       <c r="L29" s="18"/>
-      <c r="M29" s="122"/>
+      <c r="M29" s="111"/>
       <c r="N29" s="19">
-        <f>SUMIFS(B29:M29,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O29" s="19">
-        <f>SUMIFS(B29:M29,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P29" s="19">
-        <f>SUMIFS(B29:M29,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q29" s="19">
-        <f>SUMIFS(B29:M29,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R29" s="19">
-        <f>SUMIFS(B29:M29,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S29" s="19">
-        <f>SUMIFS(B29:M29,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T29" s="19">
-        <f>SUMIFS(B29:M29,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U29" s="19">
-        <f>SUMIFS(B29:M29,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V29" s="19">
-        <f>SUMIFS(B29:M29,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W29" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5542,45 +5538,45 @@
       <c r="J30" s="61"/>
       <c r="K30" s="61"/>
       <c r="L30" s="59"/>
-      <c r="M30" s="122"/>
+      <c r="M30" s="111"/>
       <c r="N30" s="60">
-        <f>SUMIFS(B30:M30,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O30" s="60">
-        <f>SUMIFS(B30:M30,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P30" s="60">
-        <f>SUMIFS(B30:M30,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q30" s="60">
-        <f>SUMIFS(B30:M30,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R30" s="60">
-        <f>SUMIFS(B30:M30,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S30" s="60">
-        <f>SUMIFS(B30:M30,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T30" s="60">
-        <f>SUMIFS(B30:M30,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U30" s="60">
-        <f>SUMIFS(B30:M30,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V30" s="60">
-        <f>SUMIFS(B30:M30,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W30" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5599,45 +5595,45 @@
       <c r="J31" s="61"/>
       <c r="K31" s="61"/>
       <c r="L31" s="59"/>
-      <c r="M31" s="122"/>
+      <c r="M31" s="111"/>
       <c r="N31" s="60">
-        <f>SUMIFS(B31:M31,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O31" s="60">
-        <f>SUMIFS(B31:M31,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P31" s="60">
-        <f>SUMIFS(B31:M31,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q31" s="60">
-        <f>SUMIFS(B31:M31,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R31" s="60">
-        <f>SUMIFS(B31:M31,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S31" s="60">
-        <f>SUMIFS(B31:M31,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T31" s="60">
-        <f>SUMIFS(B31:M31,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U31" s="60">
-        <f>SUMIFS(B31:M31,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V31" s="60">
-        <f>SUMIFS(B31:M31,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W31" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5656,45 +5652,45 @@
       <c r="J32" s="81"/>
       <c r="K32" s="81"/>
       <c r="L32" s="18"/>
-      <c r="M32" s="122"/>
+      <c r="M32" s="111"/>
       <c r="N32" s="19">
-        <f>SUMIFS(B32:M32,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O32" s="19">
-        <f>SUMIFS(B32:M32,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P32" s="19">
-        <f>SUMIFS(B32:M32,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q32" s="19">
-        <f>SUMIFS(B32:M32,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R32" s="19">
-        <f>SUMIFS(B32:M32,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S32" s="19">
-        <f>SUMIFS(B32:M32,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T32" s="19">
-        <f>SUMIFS(B32:M32,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U32" s="19">
-        <f>SUMIFS(B32:M32,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V32" s="19">
-        <f>SUMIFS(B32:M32,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W32" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5713,45 +5709,45 @@
       <c r="J33" s="81"/>
       <c r="K33" s="81"/>
       <c r="L33" s="18"/>
-      <c r="M33" s="122"/>
+      <c r="M33" s="111"/>
       <c r="N33" s="19">
-        <f>SUMIFS(B33:M33,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O33" s="19">
-        <f>SUMIFS(B33:M33,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P33" s="19">
-        <f>SUMIFS(B33:M33,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q33" s="19">
-        <f>SUMIFS(B33:M33,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R33" s="19">
-        <f>SUMIFS(B33:M33,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S33" s="19">
-        <f>SUMIFS(B33:M33,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T33" s="19">
-        <f>SUMIFS(B33:M33,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U33" s="19">
-        <f>SUMIFS(B33:M33,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V33" s="19">
-        <f>SUMIFS(B33:M33,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W33" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5770,45 +5766,45 @@
       <c r="J34" s="81"/>
       <c r="K34" s="81"/>
       <c r="L34" s="18"/>
-      <c r="M34" s="122"/>
+      <c r="M34" s="111"/>
       <c r="N34" s="19">
-        <f>SUMIFS(B34:M34,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O34" s="19">
-        <f>SUMIFS(B34:M34,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P34" s="19">
-        <f>SUMIFS(B34:M34,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q34" s="19">
-        <f>SUMIFS(B34:M34,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R34" s="19">
-        <f>SUMIFS(B34:M34,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S34" s="19">
-        <f>SUMIFS(B34:M34,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T34" s="19">
-        <f>SUMIFS(B34:M34,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U34" s="19">
-        <f>SUMIFS(B34:M34,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V34" s="19">
-        <f>SUMIFS(B34:M34,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W34" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5827,45 +5823,45 @@
       <c r="J35" s="81"/>
       <c r="K35" s="81"/>
       <c r="L35" s="18"/>
-      <c r="M35" s="122"/>
+      <c r="M35" s="111"/>
       <c r="N35" s="19">
-        <f>SUMIFS(B35:M35,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O35" s="19">
-        <f>SUMIFS(B35:M35,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P35" s="19">
-        <f>SUMIFS(B35:M35,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q35" s="19">
-        <f>SUMIFS(B35:M35,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R35" s="19">
-        <f>SUMIFS(B35:M35,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S35" s="19">
-        <f>SUMIFS(B35:M35,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T35" s="19">
-        <f>SUMIFS(B35:M35,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U35" s="19">
-        <f>SUMIFS(B35:M35,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V35" s="19">
-        <f>SUMIFS(B35:M35,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W35" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5884,45 +5880,45 @@
       <c r="J36" s="81"/>
       <c r="K36" s="81"/>
       <c r="L36" s="18"/>
-      <c r="M36" s="122"/>
+      <c r="M36" s="111"/>
       <c r="N36" s="19">
-        <f>SUMIFS(B36:M36,B$2:M$2,"DW")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O36" s="19">
-        <f>SUMIFS(B36:M36,B$2:M$2,"TW")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P36" s="19">
-        <f>SUMIFS(B36:M36,B$2:M$2,"SW")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q36" s="19">
-        <f>SUMIFS(B36:M36,B$2:M$2,"f")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R36" s="19">
-        <f>SUMIFS(B36:M36,B$2:M$2,"B")</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S36" s="19">
-        <f>SUMIFS(B36:M36,B$2:M$2,"S")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T36" s="19">
-        <f>SUMIFS(B36:M36,B$3:M$3,"WB")</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U36" s="19">
-        <f>SUMIFS(B36:M36,B$3:M$3,"AG")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V36" s="19">
-        <f>SUMIFS(B36:M36,B$3:M$3,"PB")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W36" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5931,43 +5927,43 @@
         <v>54</v>
       </c>
       <c r="B37" s="62">
-        <f t="shared" ref="B37:K37" si="1">SUM(B6:B36)</f>
+        <f t="shared" ref="B37:K37" si="10">SUM(B6:B36)</f>
         <v>471.63</v>
       </c>
       <c r="C37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>104.97</v>
       </c>
       <c r="D37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>535.24</v>
       </c>
       <c r="E37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>107.92</v>
       </c>
       <c r="F37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>241.87</v>
       </c>
       <c r="G37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>139.63</v>
       </c>
       <c r="H37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>58.8</v>
       </c>
       <c r="I37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>26.33</v>
       </c>
       <c r="J37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K37" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L37" s="62"/>
@@ -5976,43 +5972,43 @@
         <v>1686.39</v>
       </c>
       <c r="N37" s="33">
-        <f t="shared" ref="N37:V37" si="2">SUM(N6:N36)</f>
+        <f t="shared" ref="N37:V37" si="11">SUM(N6:N36)</f>
         <v>1414.7</v>
       </c>
       <c r="O37" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>271.69</v>
       </c>
       <c r="P37" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q37" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R37" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S37" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T37" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U37" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>1660.0600000000002</v>
       </c>
       <c r="V37" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>26.33</v>
       </c>
       <c r="W37" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6032,15 +6028,15 @@
       <c r="K38" s="97"/>
       <c r="L38" s="98"/>
       <c r="M38" s="53"/>
-      <c r="N38" s="131">
+      <c r="N38" s="127">
         <f>M37-(N37+O37+P37+Q37+R37+S37)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="132"/>
-      <c r="P38" s="132"/>
-      <c r="Q38" s="132"/>
-      <c r="R38" s="132"/>
-      <c r="S38" s="133"/>
+      <c r="O38" s="128"/>
+      <c r="P38" s="128"/>
+      <c r="Q38" s="128"/>
+      <c r="R38" s="128"/>
+      <c r="S38" s="129"/>
       <c r="T38" s="15"/>
       <c r="U38" s="15"/>
       <c r="V38" s="15"/>
@@ -6152,43 +6148,43 @@
         <v>36</v>
       </c>
       <c r="B41" s="102">
-        <f t="shared" ref="B41:K41" si="3">B40-B37</f>
+        <f t="shared" ref="B41:K41" si="12">B40-B37</f>
         <v>0</v>
       </c>
       <c r="C41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="D41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>102.24000000000001</v>
       </c>
       <c r="H41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>49.120000000000005</v>
       </c>
       <c r="I41" s="102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>26.130000000000003</v>
       </c>
       <c r="J41" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>241.87</v>
       </c>
       <c r="K41" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>107.92</v>
       </c>
       <c r="L41" s="75"/>
@@ -6222,13 +6218,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N38:S38"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="N1:N5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="R1:R5"/>
-    <mergeCell ref="P1:P5"/>
-    <mergeCell ref="Q1:Q5"/>
     <mergeCell ref="U1:U5"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="W1:W5"/>
@@ -6240,6 +6229,13 @@
     <mergeCell ref="S1:S5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="T1:T5"/>
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="N1:N5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="R1:R5"/>
+    <mergeCell ref="P1:P5"/>
+    <mergeCell ref="Q1:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="10" orientation="landscape"/>

</xml_diff>